<commit_message>
added new theme for ggplot2
</commit_message>
<xml_diff>
--- a/Data/Copy of Questionnaire.xlsx
+++ b/Data/Copy of Questionnaire.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Ethnobotany and Uses" sheetId="2" r:id="rId3"/>
     <sheet name="Taro pdn n constraints" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2960" uniqueCount="539">
   <si>
     <t>S/N</t>
   </si>
@@ -1646,6 +1646,12 @@
   </si>
   <si>
     <t>Humid Forest</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Long</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1869,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1999,6 +2005,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2282,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,6 +2307,7 @@
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" customWidth="1"/>
     <col min="15" max="15" width="13.140625" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" style="47" customWidth="1"/>
@@ -2329,10 +2345,12 @@
       <c r="H1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="48" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="49"/>
+      <c r="I1" s="50" t="s">
+        <v>537</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>538</v>
+      </c>
       <c r="K1" s="32" t="s">
         <v>9</v>
       </c>
@@ -2422,7 +2440,7 @@
       <c r="N2" s="11">
         <v>56</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="51">
         <v>5</v>
       </c>
       <c r="P2" s="10" t="s">
@@ -2499,7 +2517,7 @@
       <c r="N3" s="11">
         <v>40</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="51">
         <v>3</v>
       </c>
       <c r="P3" s="10">
@@ -2576,7 +2594,7 @@
       <c r="N4" s="11">
         <v>40</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="51">
         <v>3</v>
       </c>
       <c r="P4" s="10" t="s">
@@ -2653,7 +2671,7 @@
       <c r="N5" s="11">
         <v>53</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="51">
         <v>4</v>
       </c>
       <c r="P5" s="10" t="s">
@@ -2730,7 +2748,7 @@
       <c r="N6" s="11">
         <v>45</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="51">
         <v>4</v>
       </c>
       <c r="P6" s="10" t="s">
@@ -2807,7 +2825,7 @@
       <c r="N7" s="11">
         <v>40</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="51">
         <v>3</v>
       </c>
       <c r="P7" s="10" t="s">
@@ -2884,7 +2902,7 @@
       <c r="N8" s="11">
         <v>42</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="51">
         <v>3</v>
       </c>
       <c r="P8" s="10" t="s">
@@ -2961,7 +2979,7 @@
       <c r="N9" s="11">
         <v>70</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="51">
         <v>6</v>
       </c>
       <c r="P9" s="10" t="s">
@@ -3038,7 +3056,7 @@
       <c r="N10" s="11">
         <v>50</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="51">
         <v>4</v>
       </c>
       <c r="P10" s="10" t="s">
@@ -3115,7 +3133,7 @@
       <c r="N11" s="11">
         <v>53</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="51">
         <v>4</v>
       </c>
       <c r="P11" s="10" t="s">
@@ -3192,7 +3210,7 @@
       <c r="N12" s="11">
         <v>32</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="51">
         <v>2</v>
       </c>
       <c r="P12" s="10" t="s">
@@ -3269,7 +3287,7 @@
       <c r="N13" s="11">
         <v>65</v>
       </c>
-      <c r="O13" s="11">
+      <c r="O13" s="51">
         <v>6</v>
       </c>
       <c r="P13" s="10" t="s">
@@ -3346,7 +3364,7 @@
       <c r="N14" s="11">
         <v>53</v>
       </c>
-      <c r="O14" s="11">
+      <c r="O14" s="51">
         <v>4</v>
       </c>
       <c r="P14" s="10" t="s">
@@ -3423,7 +3441,7 @@
       <c r="N15" s="11">
         <v>59</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="51">
         <v>5</v>
       </c>
       <c r="P15" s="10" t="s">
@@ -3500,7 +3518,7 @@
       <c r="N16" s="11">
         <v>34</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="51">
         <v>2</v>
       </c>
       <c r="P16" s="10" t="s">
@@ -3577,7 +3595,7 @@
       <c r="N17" s="11">
         <v>56</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="51">
         <v>5</v>
       </c>
       <c r="P17" s="20" t="s">
@@ -3654,7 +3672,7 @@
       <c r="N18" s="11">
         <v>41</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="51">
         <v>3</v>
       </c>
       <c r="P18" s="20" t="s">
@@ -3731,7 +3749,7 @@
       <c r="N19" s="11">
         <v>50</v>
       </c>
-      <c r="O19" s="11">
+      <c r="O19" s="51">
         <v>4</v>
       </c>
       <c r="P19" s="20" t="s">
@@ -3808,7 +3826,7 @@
       <c r="N20" s="22">
         <v>45</v>
       </c>
-      <c r="O20" s="22">
+      <c r="O20" s="52">
         <v>4</v>
       </c>
       <c r="P20" s="20" t="s">
@@ -3867,7 +3885,7 @@
       <c r="N21" s="11">
         <v>69</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O21" s="51">
         <v>6</v>
       </c>
       <c r="P21" s="20" t="s">
@@ -3944,7 +3962,7 @@
       <c r="N22" s="11">
         <v>38</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="51">
         <v>3</v>
       </c>
       <c r="P22" s="20" t="s">
@@ -4021,7 +4039,7 @@
       <c r="N23" s="11">
         <v>25</v>
       </c>
-      <c r="O23" s="11">
+      <c r="O23" s="51">
         <v>2</v>
       </c>
       <c r="P23" s="20" t="s">
@@ -4098,7 +4116,7 @@
       <c r="N24" s="11">
         <v>89</v>
       </c>
-      <c r="O24" s="11">
+      <c r="O24" s="51">
         <v>7</v>
       </c>
       <c r="P24" s="20" t="s">
@@ -4175,7 +4193,7 @@
       <c r="N25" s="11">
         <v>67</v>
       </c>
-      <c r="O25" s="11">
+      <c r="O25" s="51">
         <v>6</v>
       </c>
       <c r="P25" s="20" t="s">
@@ -4252,7 +4270,7 @@
       <c r="N26" s="11">
         <v>60</v>
       </c>
-      <c r="O26" s="11">
+      <c r="O26" s="51">
         <v>6</v>
       </c>
       <c r="P26" s="20" t="s">
@@ -4329,7 +4347,7 @@
       <c r="N27" s="11">
         <v>70</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O27" s="51">
         <v>6</v>
       </c>
       <c r="P27" s="20" t="s">
@@ -4406,7 +4424,7 @@
       <c r="N28" s="11">
         <v>55</v>
       </c>
-      <c r="O28" s="11">
+      <c r="O28" s="51">
         <v>5</v>
       </c>
       <c r="P28" s="20" t="s">
@@ -4483,7 +4501,7 @@
       <c r="N29" s="11">
         <v>65</v>
       </c>
-      <c r="O29" s="11">
+      <c r="O29" s="51">
         <v>6</v>
       </c>
       <c r="P29" s="20" t="s">
@@ -4560,7 +4578,7 @@
       <c r="N30" s="11">
         <v>32</v>
       </c>
-      <c r="O30" s="11">
+      <c r="O30" s="51">
         <v>2</v>
       </c>
       <c r="P30" s="20" t="s">
@@ -4637,7 +4655,7 @@
       <c r="N31" s="11">
         <v>60</v>
       </c>
-      <c r="O31" s="11">
+      <c r="O31" s="51">
         <v>5</v>
       </c>
       <c r="P31" s="20" t="s">
@@ -4714,7 +4732,7 @@
       <c r="N32" s="11">
         <v>70</v>
       </c>
-      <c r="O32" s="11">
+      <c r="O32" s="51">
         <v>6</v>
       </c>
       <c r="P32" s="20" t="s">
@@ -4791,7 +4809,7 @@
       <c r="N33" s="11">
         <v>35</v>
       </c>
-      <c r="O33" s="11">
+      <c r="O33" s="51">
         <v>3</v>
       </c>
       <c r="P33" s="20" t="s">
@@ -4868,7 +4886,7 @@
       <c r="N34" s="11">
         <v>55</v>
       </c>
-      <c r="O34" s="11">
+      <c r="O34" s="51">
         <v>5</v>
       </c>
       <c r="P34" s="20" t="s">
@@ -4945,7 +4963,7 @@
       <c r="N35" s="11">
         <v>50</v>
       </c>
-      <c r="O35" s="11">
+      <c r="O35" s="51">
         <v>4</v>
       </c>
       <c r="P35" s="20" t="s">
@@ -5022,7 +5040,7 @@
       <c r="N36" s="11">
         <v>50</v>
       </c>
-      <c r="O36" s="11">
+      <c r="O36" s="51">
         <v>4</v>
       </c>
       <c r="P36" s="20" t="s">
@@ -5099,7 +5117,7 @@
       <c r="N37" s="11">
         <v>47</v>
       </c>
-      <c r="O37" s="11">
+      <c r="O37" s="51">
         <v>4</v>
       </c>
       <c r="P37" s="20" t="s">
@@ -5176,7 +5194,7 @@
       <c r="N38" s="11">
         <v>35</v>
       </c>
-      <c r="O38" s="11">
+      <c r="O38" s="51">
         <v>3</v>
       </c>
       <c r="P38" s="20" t="s">
@@ -5253,7 +5271,7 @@
       <c r="N39" s="11">
         <v>65</v>
       </c>
-      <c r="O39" s="11">
+      <c r="O39" s="51">
         <v>6</v>
       </c>
       <c r="P39" s="20" t="s">
@@ -5330,7 +5348,7 @@
       <c r="N40" s="11">
         <v>50</v>
       </c>
-      <c r="O40" s="11">
+      <c r="O40" s="51">
         <v>4</v>
       </c>
       <c r="P40" s="20" t="s">
@@ -5407,7 +5425,7 @@
       <c r="N41" s="11">
         <v>45</v>
       </c>
-      <c r="O41" s="11">
+      <c r="O41" s="51">
         <v>4</v>
       </c>
       <c r="P41" s="20" t="s">
@@ -5484,7 +5502,7 @@
       <c r="N42" s="11">
         <v>30</v>
       </c>
-      <c r="O42" s="11">
+      <c r="O42" s="51">
         <v>2</v>
       </c>
       <c r="P42" s="20" t="s">
@@ -5561,7 +5579,7 @@
       <c r="N43" s="11">
         <v>35</v>
       </c>
-      <c r="O43" s="11">
+      <c r="O43" s="51">
         <v>3</v>
       </c>
       <c r="P43" s="20" t="s">
@@ -5638,7 +5656,7 @@
       <c r="N44" s="11">
         <v>36</v>
       </c>
-      <c r="O44" s="11">
+      <c r="O44" s="51">
         <v>3</v>
       </c>
       <c r="P44" s="20" t="s">
@@ -5715,7 +5733,7 @@
       <c r="N45" s="11">
         <v>27</v>
       </c>
-      <c r="O45" s="11">
+      <c r="O45" s="51">
         <v>2</v>
       </c>
       <c r="P45" s="20" t="s">
@@ -5792,7 +5810,7 @@
       <c r="N46" s="11">
         <v>24</v>
       </c>
-      <c r="O46" s="11">
+      <c r="O46" s="51">
         <v>1</v>
       </c>
       <c r="P46" s="20" t="s">
@@ -5869,7 +5887,7 @@
       <c r="N47" s="11">
         <v>65</v>
       </c>
-      <c r="O47" s="11">
+      <c r="O47" s="51">
         <v>6</v>
       </c>
       <c r="P47" s="20" t="s">
@@ -5946,7 +5964,7 @@
       <c r="N48" s="11">
         <v>62</v>
       </c>
-      <c r="O48" s="11">
+      <c r="O48" s="51">
         <v>5</v>
       </c>
       <c r="P48" s="20" t="s">
@@ -6023,7 +6041,7 @@
       <c r="N49" s="11">
         <v>45</v>
       </c>
-      <c r="O49" s="11">
+      <c r="O49" s="51">
         <v>4</v>
       </c>
       <c r="P49" s="29" t="s">
@@ -6100,7 +6118,7 @@
       <c r="N50" s="11">
         <v>65</v>
       </c>
-      <c r="O50" s="11">
+      <c r="O50" s="51">
         <v>6</v>
       </c>
       <c r="P50" s="20" t="s">
@@ -6177,7 +6195,7 @@
       <c r="N51" s="11">
         <v>20</v>
       </c>
-      <c r="O51" s="11">
+      <c r="O51" s="51">
         <v>1</v>
       </c>
       <c r="P51" s="20" t="s">
@@ -6254,7 +6272,7 @@
       <c r="N52" s="11">
         <v>18</v>
       </c>
-      <c r="O52" s="11">
+      <c r="O52" s="51">
         <v>1</v>
       </c>
       <c r="P52" s="20" t="s">
@@ -6331,7 +6349,7 @@
       <c r="N53" s="11">
         <v>40</v>
       </c>
-      <c r="O53" s="11">
+      <c r="O53" s="51">
         <v>3</v>
       </c>
       <c r="P53" s="20" t="s">
@@ -6408,7 +6426,7 @@
       <c r="N54" s="11">
         <v>36</v>
       </c>
-      <c r="O54" s="11">
+      <c r="O54" s="51">
         <v>3</v>
       </c>
       <c r="P54" s="20" t="s">
@@ -6485,7 +6503,7 @@
       <c r="N55" s="11">
         <v>57</v>
       </c>
-      <c r="O55" s="11">
+      <c r="O55" s="51">
         <v>5</v>
       </c>
       <c r="P55" s="20" t="s">
@@ -6562,7 +6580,7 @@
       <c r="N56" s="11">
         <v>55</v>
       </c>
-      <c r="O56" s="11">
+      <c r="O56" s="51">
         <v>5</v>
       </c>
       <c r="P56" s="20" t="s">
@@ -6639,7 +6657,7 @@
       <c r="N57" s="11">
         <v>41</v>
       </c>
-      <c r="O57" s="11">
+      <c r="O57" s="51">
         <v>3</v>
       </c>
       <c r="P57" s="20" t="s">
@@ -6716,7 +6734,7 @@
       <c r="N58" s="11">
         <v>63</v>
       </c>
-      <c r="O58" s="11">
+      <c r="O58" s="51">
         <v>5</v>
       </c>
       <c r="P58" s="20" t="s">
@@ -6793,7 +6811,7 @@
       <c r="N59" s="11">
         <v>75</v>
       </c>
-      <c r="O59" s="11">
+      <c r="O59" s="51">
         <v>7</v>
       </c>
       <c r="P59" s="20" t="s">
@@ -6870,7 +6888,7 @@
       <c r="N60" s="11">
         <v>70</v>
       </c>
-      <c r="O60" s="11">
+      <c r="O60" s="51">
         <v>6</v>
       </c>
       <c r="P60" s="20" t="s">
@@ -6947,7 +6965,7 @@
       <c r="N61" s="11">
         <v>45</v>
       </c>
-      <c r="O61" s="11">
+      <c r="O61" s="51">
         <v>4</v>
       </c>
       <c r="P61" s="20" t="s">
@@ -7024,7 +7042,7 @@
       <c r="N62" s="11">
         <v>58</v>
       </c>
-      <c r="O62" s="11">
+      <c r="O62" s="51">
         <v>5</v>
       </c>
       <c r="P62" s="20" t="s">
@@ -7101,7 +7119,7 @@
       <c r="N63" s="11">
         <v>48</v>
       </c>
-      <c r="O63" s="11">
+      <c r="O63" s="51">
         <v>4</v>
       </c>
       <c r="P63" s="20" t="s">
@@ -7178,7 +7196,7 @@
       <c r="N64" s="11">
         <v>39</v>
       </c>
-      <c r="O64" s="11">
+      <c r="O64" s="51">
         <v>3</v>
       </c>
       <c r="P64" s="20" t="s">
@@ -7213,9 +7231,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I1:J1"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7257,8 +7272,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
+      <c r="I1" s="50" t="s">
+        <v>537</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>538</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -10944,7 +10962,7 @@
   <dimension ref="A1:AL64"/>
   <sheetViews>
     <sheetView topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL1" sqref="AL1"/>
+      <selection activeCell="AQ1" sqref="AQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10987,10 +11005,12 @@
       <c r="H1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="48" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="49"/>
+      <c r="I1" s="50" t="s">
+        <v>537</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>538</v>
+      </c>
       <c r="K1" s="32" t="s">
         <v>9</v>
       </c>
@@ -12093,7 +12113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -18196,9 +18216,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I1:J1"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>